<commit_message>
created 0.2.0 with GVHD observation
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-cibmtr-cadsr-vm-cs.xlsx
+++ b/docs/CodeSystem-cibmtr-cadsr-vm-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-28T11:00:43-05:00</t>
+    <t>2023-05-02T14:51:26-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>